<commit_message>
modif narratif index 97212b640069e15e07937376f491885eb0d8557b
</commit_message>
<xml_diff>
--- a/sd-modif-narratif/ig/CodeSystem-eclaire-group-characteristic-kind-code-system.xlsx
+++ b/sd-modif-narratif/ig/CodeSystem-eclaire-group-characteristic-kind-code-system.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.0</t>
+    <t>0.3.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-11T08:59:47+00:00</t>
+    <t>2024-03-14T09:56:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>